<commit_message>
Update schema: GST signatory → Client ID link, fix Director/Shareholder/Partner IDs, remove TAN from Other Registrations
- Sheet 2 (GST): Authorised Signatory now links to Individual Client ID; Name & PAN auto-populate from Client record; section header notes multiple signatories = multiple rows per GST Reg ID
- Sheet 3 (Directors): Removed redundant 'Director Record ID' UUID — DIN (auto-fetched from Individual Client) is the director identifier
- Sheet 4 (Shareholders): Renamed 'Shareholder ID' → 'Shareholding Record ID' with clear explanation of why the record-level key exists
- Sheet 5 (Partners): Renamed 'Partner Record ID' → 'Partnership Record ID' with same explanation
- Sheet 8 (Other Registrations): Removed TAN from Registration Type dropdown (TAN is already captured in Sheet 1 — Clients Master)

https://claude.ai/code/session_015qLWBh7EdHVy8TseXaWBsC
</commit_message>
<xml_diff>
--- a/CA_Client_Schema.xlsx
+++ b/CA_Client_Schema.xlsx
@@ -19,8 +19,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1 - Clients (Master)'!$A$1:$E$57</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2 - GST Registrations'!$A$1:$E$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'3 - Directors'!$A$1:$E$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2 - GST Registrations'!$A$1:$E$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'3 - Directors'!$A$1:$E$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'4 - Shareholders'!$A$1:$E$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'5 - Partners (Firm-LLP)'!$A$1:$E$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'6 - Bank Accounts'!$A$1:$E$12</definedName>
@@ -2089,7 +2089,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2533,19 +2533,19 @@
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>── AUTHORISED SIGNATORY</t>
+          <t>── AUTHORISED SIGNATORY  [One row per signatory — repeat GST Reg. ID for multiple signatories]</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="7" t="inlineStr">
         <is>
-          <t>Authorised Signatory</t>
+          <t>Signatory Client ID</t>
         </is>
       </c>
       <c r="B21" s="6" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>Link → Clients</t>
         </is>
       </c>
       <c r="C21" s="6" t="inlineStr">
@@ -2555,80 +2555,107 @@
       </c>
       <c r="D21" s="6" t="inlineStr">
         <is>
-          <t>Name of the authorised signatory for this GSTIN</t>
+          <t>Client ID of the Individual who is authorised signatory — links to their record in Sheet 1</t>
         </is>
       </c>
       <c r="E21" s="6" t="inlineStr">
         <is>
-          <t>Rajesh Gupta</t>
+          <t>auto-linked</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="inlineStr">
         <is>
+          <t>Signatory Name</t>
+        </is>
+      </c>
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+      <c r="C22" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D22" s="6" t="inlineStr">
+        <is>
+          <t>Auto-fetched from linked Client record (Legal Name)</t>
+        </is>
+      </c>
+      <c r="E22" s="6" t="inlineStr">
+        <is>
+          <t>Rajesh Gupta</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
           <t>Signatory PAN</t>
         </is>
       </c>
-      <c r="B22" s="6" t="inlineStr">
+      <c r="B23" s="6" t="inlineStr">
         <is>
           <t>Text</t>
         </is>
       </c>
-      <c r="C22" s="6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="D22" s="6" t="inlineStr">
-        <is>
-          <t>PAN of the authorised signatory</t>
-        </is>
-      </c>
-      <c r="E22" s="6" t="inlineStr">
+      <c r="C23" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D23" s="6" t="inlineStr">
+        <is>
+          <t>Auto-fetched from linked Client record (PAN)</t>
+        </is>
+      </c>
+      <c r="E23" s="6" t="inlineStr">
         <is>
           <t>ABCPG1234D</t>
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="4" t="inlineStr">
+    <row r="24">
+      <c r="A24" s="4" t="inlineStr">
         <is>
           <t>── NOTES</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="7" t="inlineStr">
+    <row r="25">
+      <c r="A25" s="7" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="B24" s="6" t="inlineStr">
+      <c r="B25" s="6" t="inlineStr">
         <is>
           <t>Long Text</t>
         </is>
       </c>
-      <c r="C24" s="6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="D24" s="6" t="inlineStr">
+      <c r="C25" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D25" s="6" t="inlineStr">
         <is>
           <t>e.g. Filing frequency, special instructions</t>
         </is>
       </c>
-      <c r="E24" s="6" t="n"/>
+      <c r="E25" s="6" t="n"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E24"/>
+  <autoFilter ref="A1:E25"/>
   <mergeCells count="5">
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A24:E24"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A23:E23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2640,7 +2667,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2686,12 +2713,12 @@
     <row r="2">
       <c r="A2" s="5" t="inlineStr">
         <is>
-          <t>Director Record ID</t>
+          <t>Company Client ID</t>
         </is>
       </c>
       <c r="B2" s="6" t="inlineStr">
         <is>
-          <t>Auto (UUID)</t>
+          <t>Link → Clients</t>
         </is>
       </c>
       <c r="C2" s="6" t="inlineStr">
@@ -2701,19 +2728,19 @@
       </c>
       <c r="D2" s="6" t="inlineStr">
         <is>
-          <t>System generated</t>
+          <t>Client ID of the Company (Constitution = Company)</t>
         </is>
       </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
-          <t>auto-generated</t>
+          <t>auto-linked</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
         <is>
-          <t>Company Client ID</t>
+          <t>Individual Client ID</t>
         </is>
       </c>
       <c r="B3" s="6" t="inlineStr">
@@ -2728,7 +2755,7 @@
       </c>
       <c r="D3" s="6" t="inlineStr">
         <is>
-          <t>Client ID of the Company (Constitution = Company)</t>
+          <t>Client ID of the Director (Constitution = Individual) — single source of truth for this person's KYC</t>
         </is>
       </c>
       <c r="E3" s="6" t="inlineStr">
@@ -2740,12 +2767,12 @@
     <row r="4">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>Individual Client ID</t>
+          <t>DIN</t>
         </is>
       </c>
       <c r="B4" s="6" t="inlineStr">
         <is>
-          <t>Link → Clients</t>
+          <t>Text (8 char)</t>
         </is>
       </c>
       <c r="C4" s="6" t="inlineStr">
@@ -2755,24 +2782,24 @@
       </c>
       <c r="D4" s="6" t="inlineStr">
         <is>
-          <t>Client ID of the Director (Constitution = Individual) — single source of truth for this person's KYC</t>
+          <t>Director Identification Number — DIN is the director's unique identifier; auto-fetched from the Individual's Client record</t>
         </is>
       </c>
       <c r="E4" s="6" t="inlineStr">
         <is>
-          <t>auto-linked</t>
+          <t>01234567</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>DIN</t>
+          <t>Designation</t>
         </is>
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
-          <t>Text (8 char)</t>
+          <t>Dropdown</t>
         </is>
       </c>
       <c r="C5" s="6" t="inlineStr">
@@ -2782,46 +2809,42 @@
       </c>
       <c r="D5" s="6" t="inlineStr">
         <is>
-          <t>Director Identification Number — auto-fetched from the Individual's Client record</t>
+          <t>Director | Managing Director | Whole-time Director | Independent Director | Nominee Director | Additional Director</t>
         </is>
       </c>
       <c r="E5" s="6" t="inlineStr">
         <is>
-          <t>01234567</t>
+          <t>Director</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="inlineStr">
-        <is>
-          <t>Designation</t>
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>Date of Appointment</t>
         </is>
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
-          <t>Dropdown</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="C6" s="6" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D6" s="6" t="inlineStr">
-        <is>
-          <t>Director | Managing Director | Whole-time Director | Independent Director | Nominee Director | Additional Director</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="n"/>
       <c r="E6" s="6" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>01/04/2015</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
         <is>
-          <t>Date of Appointment</t>
+          <t>Date of Cessation</t>
         </is>
       </c>
       <c r="B7" s="6" t="inlineStr">
@@ -2834,40 +2857,40 @@
           <t>No</t>
         </is>
       </c>
-      <c r="D7" s="6" t="n"/>
-      <c r="E7" s="6" t="inlineStr">
-        <is>
-          <t>01/04/2015</t>
-        </is>
-      </c>
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>Leave blank if currently active</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="inlineStr">
-        <is>
-          <t>Date of Cessation</t>
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>Is Active?</t>
         </is>
       </c>
       <c r="B8" s="6" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>Yes/No</t>
         </is>
       </c>
       <c r="C8" s="6" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="D8" s="6" t="inlineStr">
-        <is>
-          <t>Leave blank if currently active</t>
-        </is>
-      </c>
-      <c r="E8" s="6" t="n"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D8" s="6" t="n"/>
+      <c r="E8" s="6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="inlineStr">
-        <is>
-          <t>Is Active?</t>
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>Is KMP?</t>
         </is>
       </c>
       <c r="B9" s="6" t="inlineStr">
@@ -2877,10 +2900,14 @@
       </c>
       <c r="C9" s="6" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D9" s="6" t="n"/>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>Key Managerial Personnel</t>
+        </is>
+      </c>
       <c r="E9" s="6" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -2890,12 +2917,12 @@
     <row r="10">
       <c r="A10" s="7" t="inlineStr">
         <is>
-          <t>Is KMP?</t>
+          <t>Notes</t>
         </is>
       </c>
       <c r="B10" s="6" t="inlineStr">
         <is>
-          <t>Yes/No</t>
+          <t>Long Text</t>
         </is>
       </c>
       <c r="C10" s="6" t="inlineStr">
@@ -2903,38 +2930,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="D10" s="6" t="inlineStr">
-        <is>
-          <t>Key Managerial Personnel</t>
-        </is>
-      </c>
-      <c r="E10" s="6" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="7" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-      <c r="B11" s="6" t="inlineStr">
-        <is>
-          <t>Long Text</t>
-        </is>
-      </c>
-      <c r="C11" s="6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="D11" s="6" t="n"/>
-      <c r="E11" s="6" t="n"/>
+      <c r="D10" s="6" t="n"/>
+      <c r="E10" s="6" t="n"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E11"/>
+  <autoFilter ref="A1:E10"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2991,7 +2991,7 @@
     <row r="2">
       <c r="A2" s="5" t="inlineStr">
         <is>
-          <t>Shareholder ID</t>
+          <t>Shareholding Record ID</t>
         </is>
       </c>
       <c r="B2" s="6" t="inlineStr">
@@ -3006,7 +3006,7 @@
       </c>
       <c r="D2" s="6" t="inlineStr">
         <is>
-          <t>System generated</t>
+          <t>System-generated primary key for this shareholding record — needed because the same person can hold shares in multiple companies, and shares can be acquired in multiple tranches over time</t>
         </is>
       </c>
       <c r="E2" s="6" t="inlineStr">
@@ -3400,7 +3400,7 @@
     <row r="2">
       <c r="A2" s="5" t="inlineStr">
         <is>
-          <t>Partner Record ID</t>
+          <t>Partnership Record ID</t>
         </is>
       </c>
       <c r="B2" s="6" t="inlineStr">
@@ -3415,7 +3415,7 @@
       </c>
       <c r="D2" s="6" t="inlineStr">
         <is>
-          <t>System generated</t>
+          <t>System-generated primary key for this partnership record — needed because the same person can be a partner in multiple firms/LLPs, and profit ratios can change over time creating new records</t>
         </is>
       </c>
       <c r="E2" s="6" t="inlineStr">
@@ -4502,7 +4502,7 @@
       </c>
       <c r="D4" s="6" t="inlineStr">
         <is>
-          <t>TAN | MSME/Udyam | IEC | FSSAI | Professional Tax | Shops &amp; Estab | Trade License | Drug License | Import Export Code | Others</t>
+          <t>MSME/Udyam | IEC | FSSAI | Professional Tax | Shops &amp; Estab | Trade License | Drug License | Import Export Code | Others  [Note: TAN is captured in Sheet 1 — Clients (Master)]</t>
         </is>
       </c>
       <c r="E4" s="6" t="inlineStr">

</xml_diff>